<commit_message>
Adequação da documentação completa para diminuir a apenas 2 necessidades.
</commit_message>
<xml_diff>
--- a/Documentação ESSA AQUI/13. Lista de Características.xlsx
+++ b/Documentação ESSA AQUI/13. Lista de Características.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1901228\Desktop\OPE\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55119\Desktop\OPE\Accountico\Documentação ESSA AQUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BBA2F7-03D6-42CA-9AF2-7E4C0D3F9FEF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6945" yWindow="1170" windowWidth="13365" windowHeight="7875"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
   <si>
     <t>Caracteristicas:</t>
   </si>
@@ -104,45 +99,6 @@
     <t>Realizar controle de fornecimento das empresas</t>
   </si>
   <si>
-    <t>Geração de arquivos em padrões contábeis</t>
-  </si>
-  <si>
-    <t>Anexar arquivos importados a cadastros</t>
-  </si>
-  <si>
-    <t>Processar arquivos importados automaticamente</t>
-  </si>
-  <si>
-    <t>Importar arquivos automaticamente</t>
-  </si>
-  <si>
-    <t>Integração de arquivos contábeis ao sistema</t>
-  </si>
-  <si>
-    <t>Gerir entrada de recursos financeiros</t>
-  </si>
-  <si>
-    <t>Gerir saída de recursos financeiros</t>
-  </si>
-  <si>
-    <t>Armazenar saldo em caixa</t>
-  </si>
-  <si>
-    <t>Projetar saldo futuro</t>
-  </si>
-  <si>
-    <t>Gerenciar recursos gastos por empresa</t>
-  </si>
-  <si>
-    <t>Gerenciar recursos adquiridos</t>
-  </si>
-  <si>
-    <t>Controle de capital líquido</t>
-  </si>
-  <si>
-    <t>Definir orçamentos para serviços prestados</t>
-  </si>
-  <si>
     <t>Médio</t>
   </si>
   <si>
@@ -165,21 +121,6 @@
   </si>
   <si>
     <t>N2. Gestão financeira de Pessoa jurídica</t>
-  </si>
-  <si>
-    <t>N3. Integração de orçamentos com contabilidade</t>
-  </si>
-  <si>
-    <t>N4. Automatização de importação de arquivos contábeis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N5. Gestão de Fluxo de caixa </t>
-  </si>
-  <si>
-    <t>N6. Gestão de compras</t>
-  </si>
-  <si>
-    <t>N7. Cadastro de Orçamentos</t>
   </si>
   <si>
     <t>anna flávia saiu do grupo.</t>
@@ -188,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -226,27 +167,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF2179AF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF2179AF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF2179AF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF2179AF"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -287,99 +213,57 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FFBE0BEF"/>
-      </left>
+      <left/>
       <right/>
-      <top style="thick">
-        <color rgb="FFBE0BEF"/>
+      <top style="medium">
+        <color rgb="FF2179AF"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FFBE0BEF"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFBE0BEF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFBE0BEF"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FFBE0BEF"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFBE0BEF"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FFBE0BEF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FFBE0BEF"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FFBE0BEF"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -388,33 +272,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,11 +603,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CV42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,23 +617,23 @@
     <col min="3" max="3" width="33.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="8.140625" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:100" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
@@ -780,655 +643,516 @@
       <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="25"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="9"/>
       <c r="CV2" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="25"/>
+      <c r="A3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="25"/>
+        <v>25</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="25"/>
+        <v>25</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="25"/>
+        <v>25</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>7</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
+        <v>25</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>8</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
+      <c r="A12" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>9</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>10</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>11</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>38</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>12</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>15</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
-        <v>31</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="12"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="16"/>
       <c r="D18" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>13</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>14</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>16</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="12"/>
+      <c r="B21" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="16"/>
       <c r="D21" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>17</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="12"/>
+      <c r="B22" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="16"/>
       <c r="D22" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6">
-        <v>18</v>
-      </c>
-      <c r="B24" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6">
-        <v>19</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
-        <v>20</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
-        <v>22</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
-        <v>21</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="15"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
-        <v>23</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9">
-        <v>24</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9">
-        <v>25</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9">
-        <v>26</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="15"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6">
-        <v>27</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6">
-        <v>28</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6">
-        <v>29</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="15"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="6">
-        <v>30</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>37</v>
-      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
@@ -1439,12 +1163,11 @@
       <c r="C42" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="21">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A30:F30"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B4:C4"/>
@@ -1456,29 +1179,12 @@
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:C40"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
     <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>